<commit_message>
Split request pipeline into two separate pipelines
- Add instance id to excel configuration.
- RequestPipeline: Assembles the requests
- ResponsePipeline: Sends request to scheduler and awaits response.
- Update README.
</commit_message>
<xml_diff>
--- a/src/test/resources/ch/sbb/rssched/client/config/request_config.xlsx
+++ b/src/test/resources/ch/sbb/rssched/client/config/request_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\src\test\resources\ch\sbb\rssched\client\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F60E86-DC89-420B-ADA6-4147FF21CE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A29E5A-4CC0-47AD-B8A9-905A511372BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="1" activeTab="1" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="maintenance_slots" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>location_id</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Passenger travelling longer than this threshold are assigned a seat. Travel times below this threshold increase the total passenger count, but not the seat count.</t>
   </si>
   <si>
-    <t>runId</t>
-  </si>
-  <si>
     <t>Id of the matsim run.</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Where to store the intermediate files and the final scheduler response of the RSSChed service</t>
   </si>
   <si>
-    <t>inputDirectory</t>
-  </si>
-  <si>
     <t>outputDirectory</t>
   </si>
   <si>
@@ -298,6 +292,21 @@
   </si>
   <si>
     <t>maximal_formation_count</t>
+  </si>
+  <si>
+    <t>matsimRunId</t>
+  </si>
+  <si>
+    <t>instanceId</t>
+  </si>
+  <si>
+    <t>rss001</t>
+  </si>
+  <si>
+    <t>Id of the rssched instance to solve, which is configured in this config file.</t>
+  </si>
+  <si>
+    <t>matsimInputDirectory</t>
   </si>
 </sst>
 </file>
@@ -697,11 +706,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -715,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>13</v>
@@ -724,292 +733,290 @@
         <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>69</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7" s="7">
         <f>90 / 3.6</f>
         <v>25</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="7">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="7">
         <f>15 * 60</f>
         <v>900</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="7">
-        <v>999</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>42</v>
+      <c r="C11" s="7">
+        <v>999</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="7">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="C13" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="7">
-        <v>60</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7">
+        <v>60</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="7">
         <f>2 * 60</f>
         <v>120</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="C17" s="7">
         <f>3 * 60</f>
         <v>180</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <f>15000 * 1000</f>
         <v>15000000</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="7">
-        <v>100</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1017,16 +1024,16 @@
         <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C19" s="7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1034,16 +1041,16 @@
         <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="7">
+        <v>25</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="7">
-        <v>50</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1051,16 +1058,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="7">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1068,20 +1075,37 @@
         <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="7">
+        <v>75</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C23" s="7">
         <v>200</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>67</v>
+      <c r="D23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
+  <autoFilter ref="A1:E23" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1093,7 +1117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1133,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1121,18 +1145,18 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1146,10 +1170,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1163,10 +1187,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -1180,10 +1204,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -1221,22 +1245,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1271,15 +1295,15 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1287,10 +1311,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -1298,10 +1322,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1309,10 +1333,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1320,10 +1344,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -1331,7 +1355,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1342,10 +1366,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1353,10 +1377,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -1399,7 +1423,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1413,7 +1437,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>2</v>

</xml_diff>